<commit_message>
Jenkinste hata almamak için hooks ta excel ve scenario kapatıldı
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/ExcelFiles/SenaryoSonuclari3.xlsx
+++ b/src/test/java/ApachePOI/ExcelFiles/SenaryoSonuclari3.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="10">
   <si>
     <t>Create and Delete citizenship from excel</t>
   </si>
@@ -30,6 +30,18 @@
   </si>
   <si>
     <t>Testing database of States functionality using JDBC</t>
+  </si>
+  <si>
+    <t>Login with valid username and password</t>
+  </si>
+  <si>
+    <t>Create a country</t>
+  </si>
+  <si>
+    <t>Create country</t>
+  </si>
+  <si>
+    <t>Create country 2</t>
   </si>
 </sst>
 </file>
@@ -74,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -384,6 +396,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>